<commit_message>
added fixed/variable expenses and colours
</commit_message>
<xml_diff>
--- a/src/excelData/data.xlsx
+++ b/src/excelData/data.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3aa74cd3d2eb7fe5/Documents/Git/CashFlowViz/src/excelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{D6DAA8AF-BBE7-48AA-88BB-3766EFFB69B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD65BEE9-8BE2-41D9-82D4-068BA011136D}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="8_{D6DAA8AF-BBE7-48AA-88BB-3766EFFB69B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FE64B2F-60C2-40DB-A2F0-6109F9F51D13}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="7" xr2:uid="{19008FBA-0248-4E70-BB53-669CA22453CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{19008FBA-0248-4E70-BB53-669CA22453CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Salaries" sheetId="1" r:id="rId1"/>
     <sheet name="Banks" sheetId="2" r:id="rId2"/>
     <sheet name="BankExpenses" sheetId="6" r:id="rId3"/>
     <sheet name="Revolut" sheetId="4" r:id="rId4"/>
-    <sheet name="LukasRevolutExpenses" sheetId="8" r:id="rId5"/>
-    <sheet name="Pockets" sheetId="5" r:id="rId6"/>
-    <sheet name="PocketExpenses" sheetId="7" r:id="rId7"/>
-    <sheet name="Joint Expenses" sheetId="9" r:id="rId8"/>
+    <sheet name="Pockets" sheetId="5" r:id="rId5"/>
+    <sheet name="PocketExpenses" sheetId="7" r:id="rId6"/>
+    <sheet name="Joint Expenses" sheetId="9" r:id="rId7"/>
+    <sheet name="Nets" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="58">
   <si>
     <t>Lukas BOI</t>
   </si>
@@ -180,10 +180,43 @@
     <t>Pet Insurance</t>
   </si>
   <si>
-    <t>Three</t>
-  </si>
-  <si>
     <t>26.50</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Fixed Expense</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Revolut</t>
+  </si>
+  <si>
+    <t>Fixed Pocket</t>
+  </si>
+  <si>
+    <t>Amazon Prime</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t>Variable Expense</t>
+  </si>
+  <si>
+    <t>ThreeMobile</t>
+  </si>
+  <si>
+    <t>Net</t>
   </si>
 </sst>
 </file>
@@ -559,183 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B86840-7617-4763-B120-9C8F23078A65}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>4400</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF729050-370A-402B-81AE-E0620239CDA6}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <f>Salaries!B2</f>
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>4400</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDCC4E92-07E9-491B-A950-FA674EC57AC8}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>2000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C597C158-64ED-4091-BA6D-80EEF1BCC158}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -748,13 +608,232 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3400</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4400</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF729050-370A-402B-81AE-E0620239CDA6}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>Salaries!B2</f>
+        <v>3400</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4400</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDCC4E92-07E9-491B-A950-FA674EC57AC8}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1600</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>200</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>2000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C597C158-64ED-4091-BA6D-80EEF1BCC158}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -762,15 +841,21 @@
         <v>500</v>
       </c>
       <c r="C2">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -779,6 +864,9 @@
       </c>
       <c r="C4">
         <v>500</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -787,21 +875,205 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E850479C-7048-4FAB-B485-4D882D785C80}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B59292-C508-4AF4-BBF8-2EDC94552237}">
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>300</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -810,152 +1082,117 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B59292-C508-4AF4-BBF8-2EDC94552237}">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412CE730-E59A-4D49-AE99-E06343FC17B9}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>67</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12">
+        <v>54</v>
+      </c>
+      <c r="E8">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17">
-        <v>30</v>
+      <c r="F8" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -964,17 +1201,18 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412CE730-E59A-4D49-AE99-E06343FC17B9}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265AE67B-8D09-40A2-A1E1-42F5CB181665}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -982,50 +1220,54 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>67</v>
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>56</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1034,57 +1276,66 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265AE67B-8D09-40A2-A1E1-42F5CB181665}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D32D50-0249-4BA3-A551-DECC3C7E1A84}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
+        <f>Banks!B2-SUM(BankExpenses!B:B)-SUM(Revolut!B:B)</f>
+        <v>394</v>
+      </c>
+      <c r="C2">
+        <f>Salaries!B3-SUM(BankExpenses!C:C)-SUM(Revolut!C:C)</f>
+        <v>1430</v>
+      </c>
+      <c r="D2">
+        <f>SUM(Revolut!2:2)-SUM(Pockets!B:B)</f>
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <f>SUM(Revolut!4:4)-SUM('Joint Expenses'!B:B)</f>
+        <v>895</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>